<commit_message>
Inter users data added
Inter users data added
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -11,16 +11,19 @@
     <sheet name="EuroNormalWhitelist" sheetId="24" r:id="rId2"/>
     <sheet name="EuroReseller" sheetId="25" r:id="rId3"/>
     <sheet name="EuroMasterReseller" sheetId="26" r:id="rId4"/>
-    <sheet name="EuroNormalWhitelistGC" sheetId="21" r:id="rId5"/>
-    <sheet name="InterNormalNormallistGC" sheetId="22" r:id="rId6"/>
-    <sheet name="Transactions" sheetId="23" r:id="rId7"/>
+    <sheet name="InterNormalWhitelist" sheetId="27" r:id="rId5"/>
+    <sheet name="InterReseller" sheetId="28" r:id="rId6"/>
+    <sheet name="InterMasterReseller" sheetId="29" r:id="rId7"/>
+    <sheet name="EuroNormalWhitelistGC" sheetId="21" r:id="rId8"/>
+    <sheet name="InterNormalNormallistGC" sheetId="22" r:id="rId9"/>
+    <sheet name="Transactions" sheetId="23" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="98">
   <si>
     <t>%</t>
   </si>
@@ -253,9 +256,6 @@
     <t>International English</t>
   </si>
   <si>
-    <t>GL Tester</t>
-  </si>
-  <si>
     <t>normaltester</t>
   </si>
   <si>
@@ -299,6 +299,24 @@
   </si>
   <si>
     <t>Marka</t>
+  </si>
+  <si>
+    <t>International Normal Tester</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>International Reseller</t>
+  </si>
+  <si>
+    <t>International Master</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -709,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +736,8 @@
     <col min="1" max="1" width="47.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.42578125" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1" collapsed="1"/>
     <col min="7" max="8" width="17.140625" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="23" customWidth="1" collapsed="1"/>
@@ -786,10 +805,10 @@
         <v>75</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>19</v>
@@ -821,7 +840,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>7</v>
@@ -857,10 +876,10 @@
         <v>76</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>24</v>
@@ -886,7 +905,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>7</v>
@@ -901,16 +920,16 @@
         <v>27</v>
       </c>
       <c r="J3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="M3" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
@@ -918,10 +937,10 @@
         <v>76</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>24</v>
@@ -949,7 +968,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>7</v>
@@ -964,16 +983,16 @@
         <v>32</v>
       </c>
       <c r="J4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="L4" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
@@ -981,10 +1000,10 @@
         <v>76</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>24</v>
@@ -1014,7 +1033,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>10</v>
@@ -1038,7 +1057,7 @@
         <v>68</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="N5" s="15" t="s">
         <v>72</v>
@@ -1050,9 +1069,11 @@
         <v>76</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="R5" s="15"/>
+        <v>83</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>97</v>
+      </c>
       <c r="S5" s="5" t="s">
         <v>25</v>
       </c>
@@ -1076,7 +1097,9 @@
       <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
@@ -1103,9 +1126,15 @@
       </c>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
+      <c r="P6" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>97</v>
+      </c>
       <c r="S6" s="8" t="s">
         <v>25</v>
       </c>
@@ -1133,7 +1162,9 @@
       <c r="D7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1150,7 +1181,7 @@
         <v>65</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>68</v>
@@ -1160,9 +1191,15 @@
       </c>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
+      <c r="P7" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="S7" s="10" t="s">
         <v>25</v>
       </c>
@@ -1541,9 +1578,49 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
-  <ignoredErrors>
-    <ignoredError sqref="M5" numberStoredAsText="1"/>
-  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1689,7 +1766,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="18" t="str">
         <f>TestAccountsInfo!Q2</f>
@@ -1698,7 +1775,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="18" t="str">
         <f>TestAccountsInfo!R2</f>
@@ -1712,6 +1789,498 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="19" t="str">
+        <f>TestAccountsInfo!C3</f>
+        <v>Tester</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="str">
+        <f>TestAccountsInfo!D3</f>
+        <v>Tester13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="19" t="str">
+        <f>TestAccountsInfo!E3</f>
+        <v>GL Testing</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="str">
+        <f>TestAccountsInfo!F3</f>
+        <v>gltesting13@gmail.com</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="18" t="str">
+        <f>TestAccountsInfo!G3</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>TestAccountsInfo!H3</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="19" t="str">
+        <f>TestAccountsInfo!I3</f>
+        <v>Spain</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="19" t="str">
+        <f>TestAccountsInfo!J3</f>
+        <v>Lviv</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="19" t="str">
+        <f>TestAccountsInfo!K3</f>
+        <v>31/1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="19" t="str">
+        <f>TestAccountsInfo!L3</f>
+        <v>Marka Vovchka</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>TestAccountsInfo!M3</f>
+        <v>79016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18">
+        <f>TestAccountsInfo!N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="18">
+        <f>TestAccountsInfo!O3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P3</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>TestAccountsInfo!Q3</f>
+        <v>united kingdom</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>TestAccountsInfo!R3</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="19" t="str">
+        <f>TestAccountsInfo!C4</f>
+        <v>MasterTester</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="str">
+        <f>TestAccountsInfo!D4</f>
+        <v>Tester13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="19" t="str">
+        <f>TestAccountsInfo!E4</f>
+        <v>Master Tester</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="str">
+        <f>TestAccountsInfo!F4</f>
+        <v>gltesting13@gmail.com</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="18" t="str">
+        <f>TestAccountsInfo!G4</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>TestAccountsInfo!H4</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="19" t="str">
+        <f>TestAccountsInfo!I4</f>
+        <v>Netherlands</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="19" t="str">
+        <f>TestAccountsInfo!J4</f>
+        <v>Lviv</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="19" t="str">
+        <f>TestAccountsInfo!K4</f>
+        <v>31/1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="19" t="str">
+        <f>TestAccountsInfo!L4</f>
+        <v>Marka</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>TestAccountsInfo!M4</f>
+        <v>79016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18">
+        <f>TestAccountsInfo!N4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="18">
+        <f>TestAccountsInfo!O4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P4</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>TestAccountsInfo!Q4</f>
+        <v>united kingdom</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>TestAccountsInfo!R4</f>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="str">
+        <f>TestAccountsInfo!C5</f>
+        <v>InterNormalTester</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>TestAccountsInfo!D5</f>
+        <v>Tester13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="str">
+        <f>TestAccountsInfo!E5</f>
+        <v>International Normal Tester</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>TestAccountsInfo!F5</f>
+        <v>khikmatovaj@mail.ru</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="18" t="str">
+        <f>TestAccountsInfo!G5</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>TestAccountsInfo!H5</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="str">
+        <f>TestAccountsInfo!I5</f>
+        <v>United Arab Emirates</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="str">
+        <f>TestAccountsInfo!J5</f>
+        <v>City</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="str">
+        <f>TestAccountsInfo!K5</f>
+        <v>Full</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="str">
+        <f>TestAccountsInfo!L5</f>
+        <v>Street</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>TestAccountsInfo!M5</f>
+        <v>11111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18" t="str">
+        <f>TestAccountsInfo!N5</f>
+        <v>AED</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="18" t="str">
+        <f>TestAccountsInfo!O5</f>
+        <v>USD</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P5</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>TestAccountsInfo!Q5</f>
+        <v>united kingdom</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>TestAccountsInfo!R5</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -1730,8 +2299,8 @@
         <v>47</v>
       </c>
       <c r="B1" s="19" t="str">
-        <f>TestAccountsInfo!C3</f>
-        <v>Tester</v>
+        <f>TestAccountsInfo!C6</f>
+        <v>InterTester</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1739,7 +2308,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="19" t="str">
-        <f>TestAccountsInfo!D3</f>
+        <f>TestAccountsInfo!D6</f>
         <v>Tester13</v>
       </c>
     </row>
@@ -1748,8 +2317,8 @@
         <v>60</v>
       </c>
       <c r="B3" s="19" t="str">
-        <f>TestAccountsInfo!E3</f>
-        <v>GL Testing</v>
+        <f>TestAccountsInfo!E6</f>
+        <v>International Reseller</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1757,8 +2326,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="str">
-        <f>TestAccountsInfo!F3</f>
-        <v>gltesting13@gmail.com</v>
+        <f>TestAccountsInfo!F6</f>
+        <v>khikmatovaj@mail.ru</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1766,7 +2335,7 @@
         <v>61</v>
       </c>
       <c r="B5" s="18" t="str">
-        <f>TestAccountsInfo!G3</f>
+        <f>TestAccountsInfo!G6</f>
         <v>+380979029368</v>
       </c>
     </row>
@@ -1775,7 +2344,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="18" t="str">
-        <f>TestAccountsInfo!H3</f>
+        <f>TestAccountsInfo!H6</f>
         <v>+380979029368</v>
       </c>
     </row>
@@ -1784,8 +2353,8 @@
         <v>64</v>
       </c>
       <c r="B7" s="19" t="str">
-        <f>TestAccountsInfo!I3</f>
-        <v>Spain</v>
+        <f>TestAccountsInfo!I6</f>
+        <v>Lebanon</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1793,8 +2362,8 @@
         <v>65</v>
       </c>
       <c r="B8" s="19" t="str">
-        <f>TestAccountsInfo!J3</f>
-        <v>Lviv</v>
+        <f>TestAccountsInfo!J6</f>
+        <v>City</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1802,8 +2371,8 @@
         <v>66</v>
       </c>
       <c r="B9" s="19" t="str">
-        <f>TestAccountsInfo!K3</f>
-        <v>31/1</v>
+        <f>TestAccountsInfo!K6</f>
+        <v>Full</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1811,8 +2380,8 @@
         <v>68</v>
       </c>
       <c r="B10" s="19" t="str">
-        <f>TestAccountsInfo!L3</f>
-        <v>Marka Vovchka</v>
+        <f>TestAccountsInfo!L6</f>
+        <v>Street</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1820,8 +2389,8 @@
         <v>69</v>
       </c>
       <c r="B11" s="18" t="str">
-        <f>TestAccountsInfo!M3</f>
-        <v>79016</v>
+        <f>TestAccountsInfo!M6</f>
+        <v>00001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1829,7 +2398,7 @@
         <v>71</v>
       </c>
       <c r="B12" s="18">
-        <f>TestAccountsInfo!N3</f>
+        <f>TestAccountsInfo!N6</f>
         <v>0</v>
       </c>
     </row>
@@ -1838,7 +2407,7 @@
         <v>73</v>
       </c>
       <c r="B13" s="18">
-        <f>TestAccountsInfo!O3</f>
+        <f>TestAccountsInfo!O6</f>
         <v>0</v>
       </c>
     </row>
@@ -1847,26 +2416,26 @@
         <v>75</v>
       </c>
       <c r="B14" s="18" t="str">
-        <f>TestAccountsInfo!P3</f>
+        <f>TestAccountsInfo!P6</f>
         <v>International English</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="18" t="str">
-        <f>TestAccountsInfo!Q3</f>
+        <f>TestAccountsInfo!Q6</f>
         <v>united kingdom</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="18" t="str">
-        <f>TestAccountsInfo!R3</f>
-        <v>21</v>
+        <f>TestAccountsInfo!R6</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1875,7 +2444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -1894,8 +2463,8 @@
         <v>47</v>
       </c>
       <c r="B1" s="19" t="str">
-        <f>TestAccountsInfo!C4</f>
-        <v>MasterTester</v>
+        <f>TestAccountsInfo!C7</f>
+        <v>InterMasterTester</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1903,7 +2472,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="19" t="str">
-        <f>TestAccountsInfo!D4</f>
+        <f>TestAccountsInfo!D7</f>
         <v>Tester13</v>
       </c>
     </row>
@@ -1912,8 +2481,8 @@
         <v>60</v>
       </c>
       <c r="B3" s="19" t="str">
-        <f>TestAccountsInfo!E4</f>
-        <v>Master Tester</v>
+        <f>TestAccountsInfo!E7</f>
+        <v>International Master</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,8 +2490,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="str">
-        <f>TestAccountsInfo!F4</f>
-        <v>gltesting13@gmail.com</v>
+        <f>TestAccountsInfo!F7</f>
+        <v>khikmatovaj@mail.ru</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1930,7 +2499,7 @@
         <v>61</v>
       </c>
       <c r="B5" s="18" t="str">
-        <f>TestAccountsInfo!G4</f>
+        <f>TestAccountsInfo!G7</f>
         <v>+380979029368</v>
       </c>
     </row>
@@ -1939,7 +2508,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="18" t="str">
-        <f>TestAccountsInfo!H4</f>
+        <f>TestAccountsInfo!H7</f>
         <v>+380979029368</v>
       </c>
     </row>
@@ -1948,8 +2517,8 @@
         <v>64</v>
       </c>
       <c r="B7" s="19" t="str">
-        <f>TestAccountsInfo!I4</f>
-        <v>Netherlands</v>
+        <f>TestAccountsInfo!I7</f>
+        <v>United Arab Emirates</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1957,8 +2526,8 @@
         <v>65</v>
       </c>
       <c r="B8" s="19" t="str">
-        <f>TestAccountsInfo!J4</f>
-        <v>Lviv</v>
+        <f>TestAccountsInfo!J7</f>
+        <v>City</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1966,8 +2535,8 @@
         <v>66</v>
       </c>
       <c r="B9" s="19" t="str">
-        <f>TestAccountsInfo!K4</f>
-        <v>31/1</v>
+        <f>TestAccountsInfo!K7</f>
+        <v>Address</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1975,8 +2544,8 @@
         <v>68</v>
       </c>
       <c r="B10" s="19" t="str">
-        <f>TestAccountsInfo!L4</f>
-        <v>Marka</v>
+        <f>TestAccountsInfo!L7</f>
+        <v>Street</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1984,8 +2553,8 @@
         <v>69</v>
       </c>
       <c r="B11" s="18" t="str">
-        <f>TestAccountsInfo!M4</f>
-        <v>79016</v>
+        <f>TestAccountsInfo!M7</f>
+        <v>00001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1993,7 +2562,7 @@
         <v>71</v>
       </c>
       <c r="B12" s="18">
-        <f>TestAccountsInfo!N4</f>
+        <f>TestAccountsInfo!N7</f>
         <v>0</v>
       </c>
     </row>
@@ -2002,7 +2571,7 @@
         <v>73</v>
       </c>
       <c r="B13" s="18">
-        <f>TestAccountsInfo!O4</f>
+        <f>TestAccountsInfo!O7</f>
         <v>0</v>
       </c>
     </row>
@@ -2011,26 +2580,26 @@
         <v>75</v>
       </c>
       <c r="B14" s="18" t="str">
-        <f>TestAccountsInfo!P4</f>
+        <f>TestAccountsInfo!P7</f>
         <v>International English</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="18" t="str">
-        <f>TestAccountsInfo!Q4</f>
+        <f>TestAccountsInfo!Q7</f>
         <v>united kingdom</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="18" t="str">
-        <f>TestAccountsInfo!R4</f>
-        <v>21</v>
+        <f>TestAccountsInfo!R7</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2039,7 +2608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2184,7 +2753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2222,7 +2791,7 @@
       </c>
       <c r="B3" s="19" t="str">
         <f>TestAccountsInfo!E5</f>
-        <v>GL Tester</v>
+        <v>International Normal Tester</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2294,7 +2863,7 @@
       </c>
       <c r="B11" t="str">
         <f>TestAccountsInfo!M5</f>
-        <v>00001</v>
+        <v>11111</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2322,49 +2891,6 @@
       <c r="B14" s="18" t="str">
         <f>TestAccountsInfo!P5</f>
         <v>International English</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
International users added, sign Up started
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -310,13 +310,13 @@
     <t>International Reseller</t>
   </si>
   <si>
-    <t>International Master</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>Inter Master</t>
   </si>
 </sst>
 </file>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1072,7 @@
         <v>83</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>25</v>
@@ -1133,7 +1133,7 @@
         <v>83</v>
       </c>
       <c r="R6" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S6" s="8" t="s">
         <v>25</v>
@@ -1163,7 +1163,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>10</v>
@@ -1181,7 +1181,7 @@
         <v>65</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>68</v>
@@ -1198,7 +1198,7 @@
         <v>83</v>
       </c>
       <c r="R7" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S7" s="10" t="s">
         <v>25</v>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="B3" s="19" t="str">
         <f>TestAccountsInfo!E7</f>
-        <v>International Master</v>
+        <v>Inter Master</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sign up data providers updated
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="102">
   <si>
     <t>%</t>
   </si>
@@ -318,6 +318,18 @@
   </si>
   <si>
     <t>Inter Master</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>testUsername</t>
+  </si>
+  <si>
+    <t>testFullName</t>
+  </si>
+  <si>
+    <t>+123456789876</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1642,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1655,9 @@
       <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1658,30 +1672,32 @@
       <c r="A3" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="19" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="19" t="str">
-        <f>TestAccountsInfo!G5</f>
-        <v>+380979029368</v>
+      <c r="B5" s="18" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="19" t="str">
-        <f>TestAccountsInfo!H5</f>
-        <v>+380979029368</v>
+      <c r="B6" s="18" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1757,6 +1773,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Reseller SignUp fields added
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="105">
   <si>
     <t>%</t>
   </si>
@@ -330,13 +330,22 @@
   </si>
   <si>
     <t>testerName@test.com</t>
+  </si>
+  <si>
+    <t>BusinessName</t>
+  </si>
+  <si>
+    <t>Business name</t>
+  </si>
+  <si>
+    <t>testBusiness Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +357,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -413,7 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -436,6 +451,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -738,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,9 +785,10 @@
     <col min="20" max="20" width="12.28515625" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="11.85546875" customWidth="1" collapsed="1"/>
     <col min="23" max="23" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -838,8 +858,11 @@
       <c r="W1" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -903,8 +926,9 @@
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="7"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="21"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
@@ -966,8 +990,11 @@
       <c r="W3" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>50</v>
       </c>
@@ -1031,8 +1058,11 @@
       <c r="W4" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
@@ -1096,8 +1126,9 @@
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="21"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>52</v>
       </c>
@@ -1161,8 +1192,11 @@
       <c r="W6" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>53</v>
       </c>
@@ -1226,8 +1260,11 @@
       <c r="W7" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>54</v>
       </c>
@@ -1279,8 +1316,9 @@
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="21"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>55</v>
       </c>
@@ -1336,8 +1374,11 @@
       <c r="W9" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>56</v>
       </c>
@@ -1393,8 +1434,11 @@
       <c r="W10" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>57</v>
       </c>
@@ -1446,8 +1490,9 @@
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11" s="21"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>58</v>
       </c>
@@ -1503,8 +1548,11 @@
       <c r="W12" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>59</v>
       </c>
@@ -1558,8 +1606,11 @@
       <c r="W13" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
@@ -1639,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,6 +1822,14 @@
         <v>International English</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1779,10 +1838,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,6 +1994,15 @@
         <v>21</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="19">
+        <f>TestAccountsInfo!X2</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1943,10 +2011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,6 +2167,15 @@
         <v>21</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="19" t="str">
+        <f>TestAccountsInfo!X3</f>
+        <v>Business name</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2107,335 +2184,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="19" t="str">
-        <f>TestAccountsInfo!C4</f>
-        <v>MasterTester</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="19" t="str">
-        <f>TestAccountsInfo!D4</f>
-        <v>Tester13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="19" t="str">
-        <f>TestAccountsInfo!E4</f>
-        <v>Master Tester</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="19" t="str">
-        <f>TestAccountsInfo!F4</f>
-        <v>gltesting13@gmail.com</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="18" t="str">
-        <f>TestAccountsInfo!G4</f>
-        <v>+380979029368</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="18" t="str">
-        <f>TestAccountsInfo!H4</f>
-        <v>+380979029368</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="19" t="str">
-        <f>TestAccountsInfo!I4</f>
-        <v>Netherlands</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="19" t="str">
-        <f>TestAccountsInfo!J4</f>
-        <v>Lviv</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="19" t="str">
-        <f>TestAccountsInfo!K4</f>
-        <v>31/1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="19" t="str">
-        <f>TestAccountsInfo!L4</f>
-        <v>Marka</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="18" t="str">
-        <f>TestAccountsInfo!M4</f>
-        <v>79016</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="18">
-        <f>TestAccountsInfo!N4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="18">
-        <f>TestAccountsInfo!O4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="18" t="str">
-        <f>TestAccountsInfo!P4</f>
-        <v>International English</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="18" t="str">
-        <f>TestAccountsInfo!Q4</f>
-        <v>united kingdom</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="18" t="str">
-        <f>TestAccountsInfo!R4</f>
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="str">
-        <f>TestAccountsInfo!C5</f>
-        <v>InterNormalTester</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="str">
-        <f>TestAccountsInfo!D5</f>
-        <v>Tester13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" t="str">
-        <f>TestAccountsInfo!E5</f>
-        <v>International Normal Tester</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <f>TestAccountsInfo!F5</f>
-        <v>khikmatovaj@mail.ru</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="18" t="str">
-        <f>TestAccountsInfo!G5</f>
-        <v>+380979029368</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="18" t="str">
-        <f>TestAccountsInfo!H5</f>
-        <v>+380979029368</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" t="str">
-        <f>TestAccountsInfo!I5</f>
-        <v>United Arab Emirates</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" t="str">
-        <f>TestAccountsInfo!J5</f>
-        <v>City</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="str">
-        <f>TestAccountsInfo!K5</f>
-        <v>Full</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="str">
-        <f>TestAccountsInfo!L5</f>
-        <v>Street</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="18" t="str">
-        <f>TestAccountsInfo!M5</f>
-        <v>11111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="18" t="str">
-        <f>TestAccountsInfo!N5</f>
-        <v>AED</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="18" t="str">
-        <f>TestAccountsInfo!O5</f>
-        <v>USD</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="18" t="str">
-        <f>TestAccountsInfo!P5</f>
-        <v>International English</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="18" t="str">
-        <f>TestAccountsInfo!Q5</f>
-        <v>united kingdom</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="18" t="str">
-        <f>TestAccountsInfo!R5</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -2452,8 +2201,8 @@
         <v>47</v>
       </c>
       <c r="B1" s="19" t="str">
-        <f>TestAccountsInfo!C6</f>
-        <v>InterTester</v>
+        <f>TestAccountsInfo!C4</f>
+        <v>MasterTester</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2461,7 +2210,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="19" t="str">
-        <f>TestAccountsInfo!D6</f>
+        <f>TestAccountsInfo!D4</f>
         <v>Tester13</v>
       </c>
     </row>
@@ -2470,8 +2219,8 @@
         <v>60</v>
       </c>
       <c r="B3" s="19" t="str">
-        <f>TestAccountsInfo!E6</f>
-        <v>International Reseller</v>
+        <f>TestAccountsInfo!E4</f>
+        <v>Master Tester</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,8 +2228,8 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="str">
-        <f>TestAccountsInfo!F6</f>
-        <v>khikmatovaj@mail.ru</v>
+        <f>TestAccountsInfo!F4</f>
+        <v>gltesting13@gmail.com</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2488,7 +2237,7 @@
         <v>61</v>
       </c>
       <c r="B5" s="18" t="str">
-        <f>TestAccountsInfo!G6</f>
+        <f>TestAccountsInfo!G4</f>
         <v>+380979029368</v>
       </c>
     </row>
@@ -2497,7 +2246,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="18" t="str">
-        <f>TestAccountsInfo!H6</f>
+        <f>TestAccountsInfo!H4</f>
         <v>+380979029368</v>
       </c>
     </row>
@@ -2506,8 +2255,8 @@
         <v>64</v>
       </c>
       <c r="B7" s="19" t="str">
-        <f>TestAccountsInfo!I6</f>
-        <v>Lebanon</v>
+        <f>TestAccountsInfo!I4</f>
+        <v>Netherlands</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2515,8 +2264,8 @@
         <v>65</v>
       </c>
       <c r="B8" s="19" t="str">
-        <f>TestAccountsInfo!J6</f>
-        <v>City</v>
+        <f>TestAccountsInfo!J4</f>
+        <v>Lviv</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2524,8 +2273,8 @@
         <v>66</v>
       </c>
       <c r="B9" s="19" t="str">
-        <f>TestAccountsInfo!K6</f>
-        <v>Full</v>
+        <f>TestAccountsInfo!K4</f>
+        <v>31/1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2533,8 +2282,8 @@
         <v>68</v>
       </c>
       <c r="B10" s="19" t="str">
-        <f>TestAccountsInfo!L6</f>
-        <v>Street</v>
+        <f>TestAccountsInfo!L4</f>
+        <v>Marka</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2542,8 +2291,8 @@
         <v>69</v>
       </c>
       <c r="B11" s="18" t="str">
-        <f>TestAccountsInfo!M6</f>
-        <v>00001</v>
+        <f>TestAccountsInfo!M4</f>
+        <v>79016</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2551,7 +2300,7 @@
         <v>71</v>
       </c>
       <c r="B12" s="18">
-        <f>TestAccountsInfo!N6</f>
+        <f>TestAccountsInfo!N4</f>
         <v>0</v>
       </c>
     </row>
@@ -2560,7 +2309,7 @@
         <v>73</v>
       </c>
       <c r="B13" s="18">
-        <f>TestAccountsInfo!O6</f>
+        <f>TestAccountsInfo!O4</f>
         <v>0</v>
       </c>
     </row>
@@ -2569,7 +2318,7 @@
         <v>75</v>
       </c>
       <c r="B14" s="18" t="str">
-        <f>TestAccountsInfo!P6</f>
+        <f>TestAccountsInfo!P4</f>
         <v>International English</v>
       </c>
     </row>
@@ -2578,7 +2327,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="18" t="str">
-        <f>TestAccountsInfo!Q6</f>
+        <f>TestAccountsInfo!Q4</f>
         <v>united kingdom</v>
       </c>
     </row>
@@ -2587,8 +2336,17 @@
         <v>84</v>
       </c>
       <c r="B16" s="18" t="str">
-        <f>TestAccountsInfo!R6</f>
-        <v>0</v>
+        <f>TestAccountsInfo!R4</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="19" t="str">
+        <f>TestAccountsInfo!X4</f>
+        <v>Business name</v>
       </c>
     </row>
   </sheetData>
@@ -2597,12 +2355,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2615,6 +2373,352 @@
       <c r="A1" t="s">
         <v>47</v>
       </c>
+      <c r="B1" t="str">
+        <f>TestAccountsInfo!C5</f>
+        <v>InterNormalTester</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>TestAccountsInfo!D5</f>
+        <v>Tester13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="str">
+        <f>TestAccountsInfo!E5</f>
+        <v>International Normal Tester</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>TestAccountsInfo!F5</f>
+        <v>khikmatovaj@mail.ru</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="18" t="str">
+        <f>TestAccountsInfo!G5</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>TestAccountsInfo!H5</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="str">
+        <f>TestAccountsInfo!I5</f>
+        <v>United Arab Emirates</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="str">
+        <f>TestAccountsInfo!J5</f>
+        <v>City</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="str">
+        <f>TestAccountsInfo!K5</f>
+        <v>Full</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="str">
+        <f>TestAccountsInfo!L5</f>
+        <v>Street</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>TestAccountsInfo!M5</f>
+        <v>11111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18" t="str">
+        <f>TestAccountsInfo!N5</f>
+        <v>AED</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="18" t="str">
+        <f>TestAccountsInfo!O5</f>
+        <v>USD</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P5</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>TestAccountsInfo!Q5</f>
+        <v>united kingdom</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>TestAccountsInfo!R5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="19">
+        <f>TestAccountsInfo!X5</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="19" t="str">
+        <f>TestAccountsInfo!C6</f>
+        <v>InterTester</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="str">
+        <f>TestAccountsInfo!D6</f>
+        <v>Tester13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="19" t="str">
+        <f>TestAccountsInfo!E6</f>
+        <v>International Reseller</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="str">
+        <f>TestAccountsInfo!F6</f>
+        <v>khikmatovaj@mail.ru</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="18" t="str">
+        <f>TestAccountsInfo!G6</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>TestAccountsInfo!H6</f>
+        <v>+380979029368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="19" t="str">
+        <f>TestAccountsInfo!I6</f>
+        <v>Lebanon</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="19" t="str">
+        <f>TestAccountsInfo!J6</f>
+        <v>City</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="19" t="str">
+        <f>TestAccountsInfo!K6</f>
+        <v>Full</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="19" t="str">
+        <f>TestAccountsInfo!L6</f>
+        <v>Street</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="18" t="str">
+        <f>TestAccountsInfo!M6</f>
+        <v>00001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18">
+        <f>TestAccountsInfo!N6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="18">
+        <f>TestAccountsInfo!O6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P6</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>TestAccountsInfo!Q6</f>
+        <v>united kingdom</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>TestAccountsInfo!R6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="19" t="str">
+        <f>TestAccountsInfo!X6</f>
+        <v>Business name</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
       <c r="B1" s="19" t="str">
         <f>TestAccountsInfo!C7</f>
         <v>InterMasterTester</v>
@@ -2753,6 +2857,15 @@
       <c r="B16" s="18" t="str">
         <f>TestAccountsInfo!R7</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="19" t="str">
+        <f>TestAccountsInfo!X7</f>
+        <v>Business name</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Success SignUp added for Normal and Reseller
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TestAccountsInfo" sheetId="10" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="InterNormalNormallistGC" sheetId="22" r:id="rId9"/>
     <sheet name="Transactions" sheetId="23" r:id="rId10"/>
     <sheet name="SignUpNormalUser" sheetId="30" r:id="rId11"/>
+    <sheet name="SignUpReseller" sheetId="31" r:id="rId12"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="105">
   <si>
     <t>%</t>
   </si>
@@ -1692,6 +1693,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="str">
+        <f>TestAccountsInfo!D5</f>
+        <v>Tester13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="19" t="str">
+        <f>TestAccountsInfo!I5</f>
+        <v>United Arab Emirates</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="19" t="str">
+        <f>TestAccountsInfo!J5</f>
+        <v>City</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="19" t="str">
+        <f>TestAccountsInfo!K5</f>
+        <v>Full</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="19" t="str">
+        <f>TestAccountsInfo!L5</f>
+        <v>Street</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="str">
+        <f>TestAccountsInfo!M5</f>
+        <v>11111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="18" t="str">
+        <f>TestAccountsInfo!O5</f>
+        <v>USD</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P5</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>

</xml_diff>

<commit_message>
NormalUser deals verify added
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="TestAccountsInfo" sheetId="10" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="RecurrentEuroMasterReseller" sheetId="34" r:id="rId10"/>
     <sheet name="SignUpNormalUser" sheetId="30" r:id="rId11"/>
     <sheet name="SignUpReseller" sheetId="31" r:id="rId12"/>
+    <sheet name="NymgoNormalEuroUser" sheetId="35" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="127">
   <si>
     <t>%</t>
   </si>
@@ -391,6 +392,21 @@
   </si>
   <si>
     <t>Greece</t>
+  </si>
+  <si>
+    <t>dealtester</t>
+  </si>
+  <si>
+    <t>dealtester@mail.ru</t>
+  </si>
+  <si>
+    <t>1111111111</t>
+  </si>
+  <si>
+    <t>Deal tester</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -480,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -508,6 +524,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -812,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -2161,7 +2178,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,6 +2469,189 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="18" t="str">
+        <f>TestAccountsInfo!H9</f>
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="19" t="str">
+        <f>TestAccountsInfo!I9</f>
+        <v>Estonia</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="19" t="str">
+        <f>TestAccountsInfo!J9</f>
+        <v>City</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="19" t="str">
+        <f>TestAccountsInfo!K9</f>
+        <v>Full</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="19" t="str">
+        <f>TestAccountsInfo!L9</f>
+        <v>Street</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="18" t="str">
+        <f>TestAccountsInfo!N9</f>
+        <v>AED</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="18" t="str">
+        <f>TestAccountsInfo!O9</f>
+        <v>USD</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P9</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>TestAccountsInfo!Q9</f>
+        <v>united kingdom</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
@@ -3794,7 +3994,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
small updates for visa normal user
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -337,18 +337,12 @@
     <t>Business Name</t>
   </si>
   <si>
-    <t>iuliia.4</t>
-  </si>
-  <si>
     <t>iuliia.5</t>
   </si>
   <si>
     <t>iuliia.6</t>
   </si>
   <si>
-    <t>European Normal Tester</t>
-  </si>
-  <si>
     <t>European Reseller</t>
   </si>
   <si>
@@ -404,6 +398,12 @@
   </si>
   <si>
     <t>20</t>
+  </si>
+  <si>
+    <t>deal test account</t>
+  </si>
+  <si>
+    <t>11111111111</t>
   </si>
 </sst>
 </file>
@@ -827,7 +827,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,25 +937,25 @@
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>96</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>62</v>
@@ -967,7 +967,7 @@
         <v>65</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>69</v>
@@ -982,7 +982,7 @@
         <v>75</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>21</v>
@@ -1005,13 +1005,13 @@
         <v>19</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>96</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>7</v>
@@ -1050,7 +1050,7 @@
         <v>75</v>
       </c>
       <c r="R3" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>21</v>
@@ -1077,13 +1077,13 @@
         <v>19</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>96</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>7</v>
@@ -1122,7 +1122,7 @@
         <v>75</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>21</v>
@@ -1355,22 +1355,22 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>96</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>95</v>
@@ -1406,7 +1406,7 @@
         <v>75</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>22</v>
@@ -1423,22 +1423,22 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>96</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>99</v>
@@ -1447,7 +1447,7 @@
         <v>95</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>62</v>
@@ -1474,7 +1474,7 @@
         <v>75</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>22</v>
@@ -1495,22 +1495,22 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>96</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>99</v>
@@ -1519,7 +1519,7 @@
         <v>95</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>62</v>
@@ -1546,7 +1546,7 @@
         <v>75</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S10" s="10" t="s">
         <v>22</v>
@@ -1958,21 +1958,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F11" r:id="rId7"/>
-    <hyperlink ref="F12" r:id="rId8"/>
-    <hyperlink ref="F13" r:id="rId9"/>
-    <hyperlink ref="F14" r:id="rId10"/>
-    <hyperlink ref="F15" r:id="rId11"/>
-    <hyperlink ref="F16" r:id="rId12"/>
-    <hyperlink ref="F8" r:id="rId13"/>
-    <hyperlink ref="F9" r:id="rId14"/>
-    <hyperlink ref="F10" r:id="rId15"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F5" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F11" r:id="rId6"/>
+    <hyperlink ref="F12" r:id="rId7"/>
+    <hyperlink ref="F13" r:id="rId8"/>
+    <hyperlink ref="F14" r:id="rId9"/>
+    <hyperlink ref="F15" r:id="rId10"/>
+    <hyperlink ref="F16" r:id="rId11"/>
+    <hyperlink ref="F8" r:id="rId12"/>
+    <hyperlink ref="F9" r:id="rId13"/>
+    <hyperlink ref="F10" r:id="rId14"/>
+    <hyperlink ref="F2" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
@@ -2485,7 +2485,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2501,7 +2501,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2509,7 +2509,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2517,7 +2517,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>76</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="B1" t="str">
         <f>TestAccountsInfo!C2</f>
-        <v>iuliia.4</v>
+        <v>dealtester</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B3" t="str">
         <f>TestAccountsInfo!E2</f>
-        <v>European Normal Tester</v>
+        <v>deal test account</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B4" t="str">
         <f>TestAccountsInfo!F2</f>
-        <v>gltesting13@gmail.com</v>
+        <v>dealtester@mail.ru</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="B5" s="18" t="str">
         <f>TestAccountsInfo!G2</f>
-        <v>123456789</v>
+        <v>11111111111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="B6" s="18" t="str">
         <f>TestAccountsInfo!H2</f>
-        <v>123456789</v>
+        <v>1111111111</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="B7" t="str">
         <f>TestAccountsInfo!I2</f>
-        <v>Spain</v>
+        <v>United Kingdom</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2759,7 +2759,7 @@
       </c>
       <c r="B11" s="18" t="str">
         <f>TestAccountsInfo!M2</f>
-        <v>00001</v>
+        <v>11111</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Buy Deals for Inter and Euro resellers
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestAccountsInfo" sheetId="10" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="RecurrentEuroMasterReseller" sheetId="34" r:id="rId10"/>
     <sheet name="SignUpNormalUser" sheetId="30" r:id="rId11"/>
     <sheet name="SignUpReseller" sheetId="31" r:id="rId12"/>
-    <sheet name="NymgoNormalEuroUser" sheetId="35" r:id="rId13"/>
+    <sheet name="NymgoEuroNormalUser" sheetId="35" r:id="rId13"/>
+    <sheet name="NymgoEuroReseller" sheetId="36" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="131">
   <si>
     <t>%</t>
   </si>
@@ -404,6 +405,21 @@
   </si>
   <si>
     <t>11111111111</t>
+  </si>
+  <si>
+    <t>dealReseller</t>
+  </si>
+  <si>
+    <t>Deal Reseller Account</t>
+  </si>
+  <si>
+    <t>111111111</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
 </sst>
 </file>
@@ -826,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2649,6 +2665,187 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="19" t="str">
+        <f>TestAccountsInfo!J9</f>
+        <v>City</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="19" t="str">
+        <f>TestAccountsInfo!K9</f>
+        <v>Full</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="19" t="str">
+        <f>TestAccountsInfo!L9</f>
+        <v>Street</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="18" t="str">
+        <f>TestAccountsInfo!N9</f>
+        <v>AED</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="18" t="str">
+        <f>TestAccountsInfo!O9</f>
+        <v>USD</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="18" t="str">
+        <f>TestAccountsInfo!P9</f>
+        <v>International English</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="18" t="str">
+        <f>TestAccountsInfo!Q9</f>
+        <v>united kingdom</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>

</xml_diff>

<commit_message>
Normal user transfer credits started
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestAccountsInfo" sheetId="10" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="134">
   <si>
     <t>%</t>
   </si>
@@ -379,55 +379,58 @@
     <t>Estonia</t>
   </si>
   <si>
-    <t>dealtester@mail.ru</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
-    <t>dealReseller</t>
-  </si>
-  <si>
-    <t>Deal Reseller Account</t>
-  </si>
-  <si>
     <t>111111111</t>
   </si>
   <si>
     <t>Finland</t>
   </si>
   <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>ideal022916</t>
+  </si>
+  <si>
+    <t>deal022916</t>
+  </si>
+  <si>
+    <t>deal022916@mail.ru</t>
+  </si>
+  <si>
+    <t>ideal022916@mail.ru</t>
+  </si>
+  <si>
+    <t>edeal031416</t>
+  </si>
+  <si>
+    <t>edeal031416@mail.ru</t>
+  </si>
+  <si>
+    <t>ideal031416</t>
+  </si>
+  <si>
+    <t>ideal031416@mail.ru</t>
+  </si>
+  <si>
+    <t>idealReseller031416</t>
+  </si>
+  <si>
+    <t>idealReseller031416@mail.ru</t>
+  </si>
+  <si>
+    <t>edealReseller031416</t>
+  </si>
+  <si>
+    <t>edealReseller031416@mail.ru</t>
+  </si>
+  <si>
     <t>24</t>
-  </si>
-  <si>
-    <t>interdealtester@mail.ru</t>
-  </si>
-  <si>
-    <t>interdealreseller</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>ideal022916</t>
-  </si>
-  <si>
-    <t>deal022916</t>
-  </si>
-  <si>
-    <t>deal022916@mail.ru</t>
-  </si>
-  <si>
-    <t>ideal022916@mail.ru</t>
-  </si>
-  <si>
-    <t>deal030416</t>
-  </si>
-  <si>
-    <t>deal030416@mail.ru</t>
   </si>
 </sst>
 </file>
@@ -850,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,22 +964,22 @@
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>115</v>
@@ -1006,7 +1009,7 @@
         <v>75</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>21</v>
@@ -1074,7 +1077,7 @@
         <v>75</v>
       </c>
       <c r="R3" s="15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="S3" s="8" t="s">
         <v>21</v>
@@ -1146,7 +1149,7 @@
         <v>75</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>21</v>
@@ -1173,22 +1176,22 @@
         <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>28</v>
@@ -1430,7 +1433,7 @@
         <v>75</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>22</v>
@@ -1498,7 +1501,7 @@
         <v>75</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>22</v>
@@ -1543,7 +1546,7 @@
         <v>93</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>62</v>
@@ -1570,7 +1573,7 @@
         <v>75</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S10" s="10" t="s">
         <v>22</v>
@@ -2495,7 +2498,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2512,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2525,7 +2528,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2533,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2541,7 +2544,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,7 +2552,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2637,7 +2640,7 @@
         <v>76</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2677,14 +2680,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2692,7 +2695,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2708,7 +2711,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2716,7 +2719,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2724,7 +2727,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2732,7 +2735,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2740,7 +2743,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2819,7 +2822,7 @@
         <v>76</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2859,7 +2862,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,7 +2900,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2905,7 +2908,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2913,7 +2916,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3040,13 +3043,13 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3054,7 +3057,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3070,7 +3073,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3078,7 +3081,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3086,7 +3089,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3094,7 +3097,7 @@
         <v>60</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3102,7 +3105,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>121</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3209,6 +3212,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Accept deal alert added
</commit_message>
<xml_diff>
--- a/NymgoUsers.xlsx
+++ b/NymgoUsers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="17235" windowHeight="9525" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TestAccountsInfo" sheetId="10" r:id="rId1"/>
@@ -409,28 +409,28 @@
     <t>24</t>
   </si>
   <si>
-    <t>ideal031816</t>
-  </si>
-  <si>
-    <t>ideal031816@mail.ru</t>
-  </si>
-  <si>
-    <t>edeal031816</t>
-  </si>
-  <si>
-    <t>edeal031816@mail.ru</t>
-  </si>
-  <si>
-    <t>idealReseller031816</t>
-  </si>
-  <si>
-    <t>idealReseller031816@mail.ru</t>
-  </si>
-  <si>
-    <t>edealReseller031816</t>
-  </si>
-  <si>
-    <t>edealReseller031816@mail.ru</t>
+    <t>ideal032816</t>
+  </si>
+  <si>
+    <t>ideal032816@mail.ru</t>
+  </si>
+  <si>
+    <t>edeal032816</t>
+  </si>
+  <si>
+    <t>edeal032816@mail.ru</t>
+  </si>
+  <si>
+    <t>edealReseller032816</t>
+  </si>
+  <si>
+    <t>edealReseller032816@mail.ru</t>
+  </si>
+  <si>
+    <t>idealReseller032816</t>
+  </si>
+  <si>
+    <t>idealReseller032816@mail.ru</t>
   </si>
 </sst>
 </file>
@@ -2498,7 +2498,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2680,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2695,7 +2695,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2711,7 +2711,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3042,8 +3042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,7 +3057,7 @@
         <v>44</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3073,7 +3073,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>